<commit_message>
Add saner paper replication package.
</commit_message>
<xml_diff>
--- a/replication_package/manual_validation/manual_validation.xlsx
+++ b/replication_package/manual_validation/manual_validation.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44683271-3BB5-4EE4-9B10-8C399B3C56CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B049D0BB-E767-4610-9A18-4670D394D64F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Validation" sheetId="1" r:id="rId1"/>
@@ -1334,13 +1334,13 @@
     <t>Bugfix.</t>
   </si>
   <si>
+    <t>Finding 3</t>
+  </si>
+  <si>
     <t>Finding 4</t>
   </si>
   <si>
     <t>Other Refactorings</t>
-  </si>
-  <si>
-    <t>Finding 5</t>
   </si>
 </sst>
 </file>
@@ -1527,19 +1527,19 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1760,8 +1760,8 @@
   </sheetPr>
   <dimension ref="A1:G112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="A65" sqref="A65:A85"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A86" sqref="A86:A106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1798,7 +1798,7 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="20" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="23" t="s">
@@ -1821,8 +1821,8 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="25"/>
-      <c r="B3" s="21"/>
+      <c r="A3" s="21"/>
+      <c r="B3" s="24"/>
       <c r="C3" s="1" t="s">
         <v>14</v>
       </c>
@@ -1840,8 +1840,8 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="25"/>
-      <c r="B4" s="21"/>
+      <c r="A4" s="21"/>
+      <c r="B4" s="24"/>
       <c r="C4" s="1" t="s">
         <v>18</v>
       </c>
@@ -1859,8 +1859,8 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="25"/>
-      <c r="B5" s="20" t="s">
+      <c r="A5" s="21"/>
+      <c r="B5" s="25" t="s">
         <v>23</v>
       </c>
       <c r="C5" s="1" t="s">
@@ -1880,8 +1880,8 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="25"/>
-      <c r="B6" s="21"/>
+      <c r="A6" s="21"/>
+      <c r="B6" s="24"/>
       <c r="C6" s="1" t="s">
         <v>24</v>
       </c>
@@ -1899,8 +1899,8 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="25"/>
-      <c r="B7" s="21"/>
+      <c r="A7" s="21"/>
+      <c r="B7" s="24"/>
       <c r="C7" s="1" t="s">
         <v>31</v>
       </c>
@@ -1918,8 +1918,8 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="25"/>
-      <c r="B8" s="20" t="s">
+      <c r="A8" s="21"/>
+      <c r="B8" s="25" t="s">
         <v>36</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -1939,8 +1939,8 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="25"/>
-      <c r="B9" s="21"/>
+      <c r="A9" s="21"/>
+      <c r="B9" s="24"/>
       <c r="C9" s="1" t="s">
         <v>41</v>
       </c>
@@ -1958,8 +1958,8 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="25"/>
-      <c r="B10" s="21"/>
+      <c r="A10" s="21"/>
+      <c r="B10" s="24"/>
       <c r="C10" s="1" t="s">
         <v>44</v>
       </c>
@@ -1977,8 +1977,8 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="25"/>
-      <c r="B11" s="20" t="s">
+      <c r="A11" s="21"/>
+      <c r="B11" s="25" t="s">
         <v>49</v>
       </c>
       <c r="C11" s="1" t="s">
@@ -1998,8 +1998,8 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="25"/>
-      <c r="B12" s="21"/>
+      <c r="A12" s="21"/>
+      <c r="B12" s="24"/>
       <c r="C12" s="1" t="s">
         <v>55</v>
       </c>
@@ -2017,8 +2017,8 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="25"/>
-      <c r="B13" s="21"/>
+      <c r="A13" s="21"/>
+      <c r="B13" s="24"/>
       <c r="C13" s="1" t="s">
         <v>59</v>
       </c>
@@ -2036,8 +2036,8 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="25"/>
-      <c r="B14" s="20" t="s">
+      <c r="A14" s="21"/>
+      <c r="B14" s="25" t="s">
         <v>64</v>
       </c>
       <c r="C14" s="1" t="s">
@@ -2057,8 +2057,8 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="25"/>
-      <c r="B15" s="21"/>
+      <c r="A15" s="21"/>
+      <c r="B15" s="24"/>
       <c r="C15" s="1" t="s">
         <v>69</v>
       </c>
@@ -2076,8 +2076,8 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="25"/>
-      <c r="B16" s="21"/>
+      <c r="A16" s="21"/>
+      <c r="B16" s="24"/>
       <c r="C16" s="1" t="s">
         <v>73</v>
       </c>
@@ -2095,8 +2095,8 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="25"/>
-      <c r="B17" s="20" t="s">
+      <c r="A17" s="21"/>
+      <c r="B17" s="25" t="s">
         <v>78</v>
       </c>
       <c r="C17" s="1" t="s">
@@ -2116,8 +2116,8 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" s="25"/>
-      <c r="B18" s="21"/>
+      <c r="A18" s="21"/>
+      <c r="B18" s="24"/>
       <c r="C18" s="1" t="s">
         <v>83</v>
       </c>
@@ -2135,8 +2135,8 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="25"/>
-      <c r="B19" s="21"/>
+      <c r="A19" s="21"/>
+      <c r="B19" s="24"/>
       <c r="C19" s="1" t="s">
         <v>88</v>
       </c>
@@ -2154,8 +2154,8 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20" s="25"/>
-      <c r="B20" s="20" t="s">
+      <c r="A20" s="21"/>
+      <c r="B20" s="25" t="s">
         <v>92</v>
       </c>
       <c r="C20" s="1" t="s">
@@ -2175,8 +2175,8 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21" s="25"/>
-      <c r="B21" s="21"/>
+      <c r="A21" s="21"/>
+      <c r="B21" s="24"/>
       <c r="C21" s="1" t="s">
         <v>97</v>
       </c>
@@ -2194,8 +2194,8 @@
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A22" s="26"/>
-      <c r="B22" s="22"/>
+      <c r="A22" s="22"/>
+      <c r="B22" s="26"/>
       <c r="C22" s="1" t="s">
         <v>97</v>
       </c>
@@ -2213,7 +2213,7 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" s="24" t="s">
+      <c r="A23" s="20" t="s">
         <v>104</v>
       </c>
       <c r="B23" s="23" t="s">
@@ -2236,8 +2236,8 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A24" s="25"/>
-      <c r="B24" s="21"/>
+      <c r="A24" s="21"/>
+      <c r="B24" s="24"/>
       <c r="C24" s="1" t="s">
         <v>109</v>
       </c>
@@ -2255,8 +2255,8 @@
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A25" s="25"/>
-      <c r="B25" s="21"/>
+      <c r="A25" s="21"/>
+      <c r="B25" s="24"/>
       <c r="C25" s="1" t="s">
         <v>112</v>
       </c>
@@ -2274,8 +2274,8 @@
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A26" s="25"/>
-      <c r="B26" s="20" t="s">
+      <c r="A26" s="21"/>
+      <c r="B26" s="25" t="s">
         <v>23</v>
       </c>
       <c r="C26" s="1" t="s">
@@ -2295,8 +2295,8 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A27" s="25"/>
-      <c r="B27" s="21"/>
+      <c r="A27" s="21"/>
+      <c r="B27" s="24"/>
       <c r="C27" s="1" t="s">
         <v>121</v>
       </c>
@@ -2314,8 +2314,8 @@
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A28" s="25"/>
-      <c r="B28" s="21"/>
+      <c r="A28" s="21"/>
+      <c r="B28" s="24"/>
       <c r="C28" s="1" t="s">
         <v>125</v>
       </c>
@@ -2333,8 +2333,8 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A29" s="25"/>
-      <c r="B29" s="20" t="s">
+      <c r="A29" s="21"/>
+      <c r="B29" s="25" t="s">
         <v>36</v>
       </c>
       <c r="C29" s="1" t="s">
@@ -2354,8 +2354,8 @@
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A30" s="25"/>
-      <c r="B30" s="21"/>
+      <c r="A30" s="21"/>
+      <c r="B30" s="24"/>
       <c r="C30" s="1" t="s">
         <v>133</v>
       </c>
@@ -2373,8 +2373,8 @@
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A31" s="25"/>
-      <c r="B31" s="21"/>
+      <c r="A31" s="21"/>
+      <c r="B31" s="24"/>
       <c r="C31" s="1" t="s">
         <v>136</v>
       </c>
@@ -2392,8 +2392,8 @@
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A32" s="25"/>
-      <c r="B32" s="20" t="s">
+      <c r="A32" s="21"/>
+      <c r="B32" s="25" t="s">
         <v>49</v>
       </c>
       <c r="C32" s="1" t="s">
@@ -2413,8 +2413,8 @@
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A33" s="25"/>
-      <c r="B33" s="21"/>
+      <c r="A33" s="21"/>
+      <c r="B33" s="24"/>
       <c r="C33" s="1" t="s">
         <v>144</v>
       </c>
@@ -2432,8 +2432,8 @@
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A34" s="25"/>
-      <c r="B34" s="21"/>
+      <c r="A34" s="21"/>
+      <c r="B34" s="24"/>
       <c r="C34" s="1" t="s">
         <v>148</v>
       </c>
@@ -2451,8 +2451,8 @@
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A35" s="25"/>
-      <c r="B35" s="20" t="s">
+      <c r="A35" s="21"/>
+      <c r="B35" s="25" t="s">
         <v>64</v>
       </c>
       <c r="C35" s="1" t="s">
@@ -2472,8 +2472,8 @@
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A36" s="25"/>
-      <c r="B36" s="21"/>
+      <c r="A36" s="21"/>
+      <c r="B36" s="24"/>
       <c r="C36" s="1" t="s">
         <v>156</v>
       </c>
@@ -2491,8 +2491,8 @@
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A37" s="25"/>
-      <c r="B37" s="21"/>
+      <c r="A37" s="21"/>
+      <c r="B37" s="24"/>
       <c r="C37" s="1" t="s">
         <v>160</v>
       </c>
@@ -2510,8 +2510,8 @@
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A38" s="25"/>
-      <c r="B38" s="20" t="s">
+      <c r="A38" s="21"/>
+      <c r="B38" s="25" t="s">
         <v>78</v>
       </c>
       <c r="C38" s="1" t="s">
@@ -2531,8 +2531,8 @@
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A39" s="25"/>
-      <c r="B39" s="21"/>
+      <c r="A39" s="21"/>
+      <c r="B39" s="24"/>
       <c r="C39" s="1" t="s">
         <v>167</v>
       </c>
@@ -2550,8 +2550,8 @@
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A40" s="25"/>
-      <c r="B40" s="21"/>
+      <c r="A40" s="21"/>
+      <c r="B40" s="24"/>
       <c r="C40" s="1" t="s">
         <v>171</v>
       </c>
@@ -2569,8 +2569,8 @@
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A41" s="25"/>
-      <c r="B41" s="20" t="s">
+      <c r="A41" s="21"/>
+      <c r="B41" s="25" t="s">
         <v>92</v>
       </c>
       <c r="C41" s="1" t="s">
@@ -2590,8 +2590,8 @@
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A42" s="25"/>
-      <c r="B42" s="21"/>
+      <c r="A42" s="21"/>
+      <c r="B42" s="24"/>
       <c r="C42" s="1" t="s">
         <v>178</v>
       </c>
@@ -2609,8 +2609,8 @@
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A43" s="26"/>
-      <c r="B43" s="22"/>
+      <c r="A43" s="22"/>
+      <c r="B43" s="26"/>
       <c r="C43" s="1" t="s">
         <v>181</v>
       </c>
@@ -2628,7 +2628,7 @@
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A44" s="24" t="s">
+      <c r="A44" s="20" t="s">
         <v>439</v>
       </c>
       <c r="B44" s="23" t="s">
@@ -2651,8 +2651,8 @@
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A45" s="25"/>
-      <c r="B45" s="21"/>
+      <c r="A45" s="21"/>
+      <c r="B45" s="24"/>
       <c r="C45" s="1" t="s">
         <v>190</v>
       </c>
@@ -2670,8 +2670,8 @@
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A46" s="25"/>
-      <c r="B46" s="21"/>
+      <c r="A46" s="21"/>
+      <c r="B46" s="24"/>
       <c r="C46" s="1" t="s">
         <v>195</v>
       </c>
@@ -2689,8 +2689,8 @@
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A47" s="25"/>
-      <c r="B47" s="20" t="s">
+      <c r="A47" s="21"/>
+      <c r="B47" s="25" t="s">
         <v>23</v>
       </c>
       <c r="C47" s="1" t="s">
@@ -2710,8 +2710,8 @@
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A48" s="25"/>
-      <c r="B48" s="21"/>
+      <c r="A48" s="21"/>
+      <c r="B48" s="24"/>
       <c r="C48" s="1" t="s">
         <v>205</v>
       </c>
@@ -2729,8 +2729,8 @@
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A49" s="25"/>
-      <c r="B49" s="21"/>
+      <c r="A49" s="21"/>
+      <c r="B49" s="24"/>
       <c r="C49" s="1" t="s">
         <v>208</v>
       </c>
@@ -2748,8 +2748,8 @@
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A50" s="25"/>
-      <c r="B50" s="20" t="s">
+      <c r="A50" s="21"/>
+      <c r="B50" s="25" t="s">
         <v>36</v>
       </c>
       <c r="C50" s="1" t="s">
@@ -2769,8 +2769,8 @@
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A51" s="25"/>
-      <c r="B51" s="21"/>
+      <c r="A51" s="21"/>
+      <c r="B51" s="24"/>
       <c r="C51" s="1" t="s">
         <v>218</v>
       </c>
@@ -2788,8 +2788,8 @@
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A52" s="25"/>
-      <c r="B52" s="21"/>
+      <c r="A52" s="21"/>
+      <c r="B52" s="24"/>
       <c r="C52" s="1" t="s">
         <v>223</v>
       </c>
@@ -2807,8 +2807,8 @@
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A53" s="25"/>
-      <c r="B53" s="20" t="s">
+      <c r="A53" s="21"/>
+      <c r="B53" s="25" t="s">
         <v>49</v>
       </c>
       <c r="C53" s="1" t="s">
@@ -2828,8 +2828,8 @@
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A54" s="25"/>
-      <c r="B54" s="21"/>
+      <c r="A54" s="21"/>
+      <c r="B54" s="24"/>
       <c r="C54" s="1" t="s">
         <v>232</v>
       </c>
@@ -2847,8 +2847,8 @@
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A55" s="25"/>
-      <c r="B55" s="21"/>
+      <c r="A55" s="21"/>
+      <c r="B55" s="24"/>
       <c r="C55" s="1" t="s">
         <v>237</v>
       </c>
@@ -2866,8 +2866,8 @@
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A56" s="25"/>
-      <c r="B56" s="20" t="s">
+      <c r="A56" s="21"/>
+      <c r="B56" s="25" t="s">
         <v>64</v>
       </c>
       <c r="C56" s="1" t="s">
@@ -2887,8 +2887,8 @@
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A57" s="25"/>
-      <c r="B57" s="21"/>
+      <c r="A57" s="21"/>
+      <c r="B57" s="24"/>
       <c r="C57" s="1" t="s">
         <v>247</v>
       </c>
@@ -2906,8 +2906,8 @@
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A58" s="25"/>
-      <c r="B58" s="21"/>
+      <c r="A58" s="21"/>
+      <c r="B58" s="24"/>
       <c r="C58" s="1" t="s">
         <v>252</v>
       </c>
@@ -2925,8 +2925,8 @@
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A59" s="25"/>
-      <c r="B59" s="20" t="s">
+      <c r="A59" s="21"/>
+      <c r="B59" s="25" t="s">
         <v>78</v>
       </c>
       <c r="C59" s="1" t="s">
@@ -2946,8 +2946,8 @@
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A60" s="25"/>
-      <c r="B60" s="21"/>
+      <c r="A60" s="21"/>
+      <c r="B60" s="24"/>
       <c r="C60" s="1" t="s">
         <v>261</v>
       </c>
@@ -2965,8 +2965,8 @@
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A61" s="25"/>
-      <c r="B61" s="21"/>
+      <c r="A61" s="21"/>
+      <c r="B61" s="24"/>
       <c r="C61" s="1" t="s">
         <v>265</v>
       </c>
@@ -2984,8 +2984,8 @@
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A62" s="25"/>
-      <c r="B62" s="20" t="s">
+      <c r="A62" s="21"/>
+      <c r="B62" s="25" t="s">
         <v>92</v>
       </c>
       <c r="C62" s="1" t="s">
@@ -3005,8 +3005,8 @@
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A63" s="25"/>
-      <c r="B63" s="21"/>
+      <c r="A63" s="21"/>
+      <c r="B63" s="24"/>
       <c r="C63" s="1" t="s">
         <v>275</v>
       </c>
@@ -3024,8 +3024,8 @@
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A64" s="26"/>
-      <c r="B64" s="22"/>
+      <c r="A64" s="22"/>
+      <c r="B64" s="26"/>
       <c r="C64" s="1" t="s">
         <v>280</v>
       </c>
@@ -3043,8 +3043,8 @@
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A65" s="24" t="s">
-        <v>441</v>
+      <c r="A65" s="20" t="s">
+        <v>440</v>
       </c>
       <c r="B65" s="23" t="s">
         <v>8</v>
@@ -3066,8 +3066,8 @@
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A66" s="25"/>
-      <c r="B66" s="21"/>
+      <c r="A66" s="21"/>
+      <c r="B66" s="24"/>
       <c r="C66" s="1" t="s">
         <v>290</v>
       </c>
@@ -3085,8 +3085,8 @@
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A67" s="25"/>
-      <c r="B67" s="21"/>
+      <c r="A67" s="21"/>
+      <c r="B67" s="24"/>
       <c r="C67" s="1" t="s">
         <v>295</v>
       </c>
@@ -3104,8 +3104,8 @@
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A68" s="25"/>
-      <c r="B68" s="20" t="s">
+      <c r="A68" s="21"/>
+      <c r="B68" s="25" t="s">
         <v>23</v>
       </c>
       <c r="C68" s="1" t="s">
@@ -3125,8 +3125,8 @@
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A69" s="25"/>
-      <c r="B69" s="21"/>
+      <c r="A69" s="21"/>
+      <c r="B69" s="24"/>
       <c r="C69" s="1" t="s">
         <v>305</v>
       </c>
@@ -3144,8 +3144,8 @@
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A70" s="25"/>
-      <c r="B70" s="21"/>
+      <c r="A70" s="21"/>
+      <c r="B70" s="24"/>
       <c r="C70" s="1" t="s">
         <v>310</v>
       </c>
@@ -3163,8 +3163,8 @@
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A71" s="25"/>
-      <c r="B71" s="20" t="s">
+      <c r="A71" s="21"/>
+      <c r="B71" s="25" t="s">
         <v>36</v>
       </c>
       <c r="C71" s="1" t="s">
@@ -3184,8 +3184,8 @@
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A72" s="25"/>
-      <c r="B72" s="21"/>
+      <c r="A72" s="21"/>
+      <c r="B72" s="24"/>
       <c r="C72" s="1" t="s">
         <v>315</v>
       </c>
@@ -3203,8 +3203,8 @@
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A73" s="25"/>
-      <c r="B73" s="21"/>
+      <c r="A73" s="21"/>
+      <c r="B73" s="24"/>
       <c r="C73" s="1" t="s">
         <v>315</v>
       </c>
@@ -3222,8 +3222,8 @@
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A74" s="25"/>
-      <c r="B74" s="20" t="s">
+      <c r="A74" s="21"/>
+      <c r="B74" s="25" t="s">
         <v>49</v>
       </c>
       <c r="C74" s="1" t="s">
@@ -3243,8 +3243,8 @@
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A75" s="25"/>
-      <c r="B75" s="21"/>
+      <c r="A75" s="21"/>
+      <c r="B75" s="24"/>
       <c r="C75" s="1" t="s">
         <v>321</v>
       </c>
@@ -3262,8 +3262,8 @@
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A76" s="25"/>
-      <c r="B76" s="21"/>
+      <c r="A76" s="21"/>
+      <c r="B76" s="24"/>
       <c r="C76" s="1" t="s">
         <v>326</v>
       </c>
@@ -3281,8 +3281,8 @@
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A77" s="25"/>
-      <c r="B77" s="20" t="s">
+      <c r="A77" s="21"/>
+      <c r="B77" s="25" t="s">
         <v>64</v>
       </c>
       <c r="C77" s="1" t="s">
@@ -3302,8 +3302,8 @@
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A78" s="25"/>
-      <c r="B78" s="21"/>
+      <c r="A78" s="21"/>
+      <c r="B78" s="24"/>
       <c r="C78" s="1" t="s">
         <v>336</v>
       </c>
@@ -3321,8 +3321,8 @@
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A79" s="25"/>
-      <c r="B79" s="21"/>
+      <c r="A79" s="21"/>
+      <c r="B79" s="24"/>
       <c r="C79" s="1" t="s">
         <v>340</v>
       </c>
@@ -3340,8 +3340,8 @@
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A80" s="25"/>
-      <c r="B80" s="20" t="s">
+      <c r="A80" s="21"/>
+      <c r="B80" s="25" t="s">
         <v>78</v>
       </c>
       <c r="C80" s="1" t="s">
@@ -3361,8 +3361,8 @@
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A81" s="25"/>
-      <c r="B81" s="21"/>
+      <c r="A81" s="21"/>
+      <c r="B81" s="24"/>
       <c r="C81" s="1" t="s">
         <v>350</v>
       </c>
@@ -3380,8 +3380,8 @@
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A82" s="25"/>
-      <c r="B82" s="21"/>
+      <c r="A82" s="21"/>
+      <c r="B82" s="24"/>
       <c r="C82" s="1" t="s">
         <v>354</v>
       </c>
@@ -3399,8 +3399,8 @@
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A83" s="25"/>
-      <c r="B83" s="20" t="s">
+      <c r="A83" s="21"/>
+      <c r="B83" s="25" t="s">
         <v>92</v>
       </c>
       <c r="C83" s="1" t="s">
@@ -3420,8 +3420,8 @@
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A84" s="25"/>
-      <c r="B84" s="21"/>
+      <c r="A84" s="21"/>
+      <c r="B84" s="24"/>
       <c r="C84" s="1" t="s">
         <v>315</v>
       </c>
@@ -3439,8 +3439,8 @@
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A85" s="26"/>
-      <c r="B85" s="22"/>
+      <c r="A85" s="22"/>
+      <c r="B85" s="26"/>
       <c r="C85" s="1" t="s">
         <v>315</v>
       </c>
@@ -3458,8 +3458,8 @@
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A86" s="24" t="s">
-        <v>440</v>
+      <c r="A86" s="20" t="s">
+        <v>441</v>
       </c>
       <c r="B86" s="23" t="s">
         <v>8</v>
@@ -3481,8 +3481,8 @@
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A87" s="25"/>
-      <c r="B87" s="21"/>
+      <c r="A87" s="21"/>
+      <c r="B87" s="24"/>
       <c r="C87" s="1" t="s">
         <v>315</v>
       </c>
@@ -3500,8 +3500,8 @@
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A88" s="25"/>
-      <c r="B88" s="21"/>
+      <c r="A88" s="21"/>
+      <c r="B88" s="24"/>
       <c r="C88" s="1" t="s">
         <v>315</v>
       </c>
@@ -3519,8 +3519,8 @@
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A89" s="25"/>
-      <c r="B89" s="20" t="s">
+      <c r="A89" s="21"/>
+      <c r="B89" s="25" t="s">
         <v>23</v>
       </c>
       <c r="C89" s="1" t="s">
@@ -3540,8 +3540,8 @@
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A90" s="25"/>
-      <c r="B90" s="21"/>
+      <c r="A90" s="21"/>
+      <c r="B90" s="24"/>
       <c r="C90" s="1" t="s">
         <v>364</v>
       </c>
@@ -3559,8 +3559,8 @@
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A91" s="25"/>
-      <c r="B91" s="21"/>
+      <c r="A91" s="21"/>
+      <c r="B91" s="24"/>
       <c r="C91" s="1" t="s">
         <v>369</v>
       </c>
@@ -3578,8 +3578,8 @@
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A92" s="25"/>
-      <c r="B92" s="20" t="s">
+      <c r="A92" s="21"/>
+      <c r="B92" s="25" t="s">
         <v>36</v>
       </c>
       <c r="C92" s="1" t="s">
@@ -3599,8 +3599,8 @@
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A93" s="25"/>
-      <c r="B93" s="21"/>
+      <c r="A93" s="21"/>
+      <c r="B93" s="24"/>
       <c r="C93" s="1" t="s">
         <v>378</v>
       </c>
@@ -3618,8 +3618,8 @@
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A94" s="25"/>
-      <c r="B94" s="21"/>
+      <c r="A94" s="21"/>
+      <c r="B94" s="24"/>
       <c r="C94" s="1" t="s">
         <v>378</v>
       </c>
@@ -3637,8 +3637,8 @@
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A95" s="25"/>
-      <c r="B95" s="20" t="s">
+      <c r="A95" s="21"/>
+      <c r="B95" s="25" t="s">
         <v>49</v>
       </c>
       <c r="C95" s="1" t="s">
@@ -3658,8 +3658,8 @@
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A96" s="25"/>
-      <c r="B96" s="21"/>
+      <c r="A96" s="21"/>
+      <c r="B96" s="24"/>
       <c r="C96" s="1" t="s">
         <v>59</v>
       </c>
@@ -3677,8 +3677,8 @@
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A97" s="25"/>
-      <c r="B97" s="21"/>
+      <c r="A97" s="21"/>
+      <c r="B97" s="24"/>
       <c r="C97" s="1" t="s">
         <v>395</v>
       </c>
@@ -3696,8 +3696,8 @@
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A98" s="25"/>
-      <c r="B98" s="20" t="s">
+      <c r="A98" s="21"/>
+      <c r="B98" s="25" t="s">
         <v>64</v>
       </c>
       <c r="C98" s="1" t="s">
@@ -3717,8 +3717,8 @@
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A99" s="25"/>
-      <c r="B99" s="21"/>
+      <c r="A99" s="21"/>
+      <c r="B99" s="24"/>
       <c r="C99" s="1" t="s">
         <v>405</v>
       </c>
@@ -3736,8 +3736,8 @@
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A100" s="25"/>
-      <c r="B100" s="21"/>
+      <c r="A100" s="21"/>
+      <c r="B100" s="24"/>
       <c r="C100" s="1" t="s">
         <v>410</v>
       </c>
@@ -3755,8 +3755,8 @@
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A101" s="25"/>
-      <c r="B101" s="20" t="s">
+      <c r="A101" s="21"/>
+      <c r="B101" s="25" t="s">
         <v>78</v>
       </c>
       <c r="C101" s="1" t="s">
@@ -3776,8 +3776,8 @@
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A102" s="25"/>
-      <c r="B102" s="21"/>
+      <c r="A102" s="21"/>
+      <c r="B102" s="24"/>
       <c r="C102" s="1" t="s">
         <v>420</v>
       </c>
@@ -3795,8 +3795,8 @@
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A103" s="25"/>
-      <c r="B103" s="21"/>
+      <c r="A103" s="21"/>
+      <c r="B103" s="24"/>
       <c r="C103" s="1" t="s">
         <v>424</v>
       </c>
@@ -3814,8 +3814,8 @@
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A104" s="25"/>
-      <c r="B104" s="20" t="s">
+      <c r="A104" s="21"/>
+      <c r="B104" s="25" t="s">
         <v>92</v>
       </c>
       <c r="C104" s="1" t="s">
@@ -3835,8 +3835,8 @@
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A105" s="25"/>
-      <c r="B105" s="21"/>
+      <c r="A105" s="21"/>
+      <c r="B105" s="24"/>
       <c r="C105" s="1" t="s">
         <v>434</v>
       </c>
@@ -3854,8 +3854,8 @@
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A106" s="26"/>
-      <c r="B106" s="22"/>
+      <c r="A106" s="22"/>
+      <c r="B106" s="26"/>
       <c r="C106" s="15" t="s">
         <v>434</v>
       </c>
@@ -3892,36 +3892,6 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="A2:A22"/>
-    <mergeCell ref="A23:A43"/>
-    <mergeCell ref="A44:A64"/>
-    <mergeCell ref="A65:A85"/>
-    <mergeCell ref="A86:A106"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="B17:B19"/>
-    <mergeCell ref="B20:B22"/>
-    <mergeCell ref="B23:B25"/>
-    <mergeCell ref="B26:B28"/>
-    <mergeCell ref="B29:B31"/>
-    <mergeCell ref="B32:B34"/>
-    <mergeCell ref="B35:B37"/>
-    <mergeCell ref="B38:B40"/>
-    <mergeCell ref="B41:B43"/>
-    <mergeCell ref="B44:B46"/>
-    <mergeCell ref="B47:B49"/>
-    <mergeCell ref="B50:B52"/>
-    <mergeCell ref="B53:B55"/>
-    <mergeCell ref="B56:B58"/>
-    <mergeCell ref="B59:B61"/>
-    <mergeCell ref="B62:B64"/>
-    <mergeCell ref="B86:B88"/>
-    <mergeCell ref="B89:B91"/>
-    <mergeCell ref="B92:B94"/>
-    <mergeCell ref="B95:B97"/>
     <mergeCell ref="B98:B100"/>
     <mergeCell ref="B101:B103"/>
     <mergeCell ref="B104:B106"/>
@@ -3932,6 +3902,36 @@
     <mergeCell ref="B77:B79"/>
     <mergeCell ref="B80:B82"/>
     <mergeCell ref="B83:B85"/>
+    <mergeCell ref="B62:B64"/>
+    <mergeCell ref="B86:B88"/>
+    <mergeCell ref="B89:B91"/>
+    <mergeCell ref="B92:B94"/>
+    <mergeCell ref="B95:B97"/>
+    <mergeCell ref="B47:B49"/>
+    <mergeCell ref="B50:B52"/>
+    <mergeCell ref="B53:B55"/>
+    <mergeCell ref="B56:B58"/>
+    <mergeCell ref="B59:B61"/>
+    <mergeCell ref="B32:B34"/>
+    <mergeCell ref="B35:B37"/>
+    <mergeCell ref="B38:B40"/>
+    <mergeCell ref="B41:B43"/>
+    <mergeCell ref="B44:B46"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="B20:B22"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="B26:B28"/>
+    <mergeCell ref="B29:B31"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="A2:A22"/>
+    <mergeCell ref="A23:A43"/>
+    <mergeCell ref="A44:A64"/>
+    <mergeCell ref="A65:A85"/>
+    <mergeCell ref="A86:A106"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>